<commit_message>
Vanilla Plants Expanded 업데이트
</commit_message>
<xml_diff>
--- a/Pull Request Here/Vanilla Plants Expanded - 2134308522/Vanilla Plants Expanded - 2134308522.xlsx
+++ b/Pull Request Here/Vanilla Plants Expanded - 2134308522/Vanilla Plants Expanded - 2134308522.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PDSSO2\Desktop\RimworldExtractor-Standard\RIM EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9AFA18-9A30-4E73-BFBB-2FC57E2DFEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124481F2-D9F8-46A0-AEC0-0C895592FFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="528">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1074,10 +1074,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>푸룬이라고도 불리는 건자두입니다. 오랫동안 상하지 않고 먹을 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>가지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1182,10 +1178,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>작고 붉은 열매로 알려진 월귤입니다. 생으로도 종종 먹으며 신맛과 밍밍한 맛이 나지만, 요리하면 자연스러운 단맛이 나오고 훨씬 더 맛있게 먹을 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>pea plant</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1254,10 +1246,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>자주빛이 도는 붉은색의 달콤한 버찌입니다. 체리로도 불리는 버찌는 계절성 겨울철 시즌이 필요하기 때문에, 추운 북방 문화권에서 인기 있는 과일이 되었습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>자두 나무</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1266,10 +1254,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>맛있고 윤기 나는 빨간 사과입니다. 사과는 인류 초기부터 간식, 디저트 재료, 그리고 과일주를 만드는 데 사용되었습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>pear tree</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1290,10 +1274,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>완두는 물이 많이 필요하여 비가 오면 크게 자랍니다. 또한, 완두콩은 두꺼운 꼬투리 만큼 긴 보존 기간을 가지는 것으로 유명합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 평소에는 다른 작물보다 효율이 떨어지지만, 비가 올 때는 성장 속도가 50% 증가합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>분홍빛의 멜론같은 식용 과일로, 오래전부터 사막 지역의 원주민들의 간식뿐만이 아니라 민간요법으로도 사용되었습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1370,18 +1350,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>약간 단단한 잎이 많은 녹색 채소로, 종종 잘게 썰어 발효시키거나 조리하여 사용됩니다. 샐러드와 코울슬로가 대표적인 요리입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>재배된 풀입니다. 약간의 빛과 최소한의 양분만 있다면 어디서나 자라는 풀입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 건초와 마찬가지로 소에게 먹일 수 있어 사실 잡초까지는 아닙니다. 병충해의 영향을 받지 않지만, 건초처럼 수확하여 보관할 수는 없습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>재배된 키 큰 풀입니다. 통과할 때 느려지고, 약간의 빛과 최소한의 양분만 있다면 어디서나 자라는 풀입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 건초와 마찬가지로 소에게 먹일 수 있어 사실 잡초까지는 아닙니다. 병충해의 영향을 받지 않지만, 건초처럼 수확하여 보관할 수는 없습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>chioggia beet plant</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1462,10 +1430,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>즙이 많고 광택이 나는 연한 붉은 과일로, 일반적으로 채소로 사용됩니다. 강하게 졸이면 내부의 산성이 부드러워져 감칠맛이 잘 느껴집니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>red beefsteak tomatoes</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1494,10 +1458,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>윤기 나는 빨간 사과를 맺는 나무로, 다양한 품종이 존재하지만 이 빨간 품종은 따뜻한 여름과 온화한 겨울을 선호합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>sakura tree</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1602,14 +1562,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>특유의 다소 떫은 맛을 가지고 있어 요리, 특히 과일 보존식품과 잼에 널리 사용됩니다. 많은 문화권에서는 자두를 건조시켜 유통기한이 긴 말린 자두로 만듭니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt;상온에서 약 15일이 지나면 장기간 유통 가능한 말린 자두가 됩니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>진한 보랏빛이 도는 매끈한 과일로 특히 신맛이 납니다. 다양한 잼, 젤리, 과일주로 만들어 먹기도 하며, 장기 보존을 위해 말려 건자두로 만들기도 합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt;상온에 두고 약 15일이 지나면 장기간 보관할 수 있는 말린 자두가 됩니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>gros michel banana tree</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1634,38 +1586,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>이 바나나 나무는 21세기에 멸종이 일어날 뻔한 대규모 바나나병 감염 사태에서도 살아남도록 유전자 변형되었습니다. 이 품종도 한 번에 전체 "송이"를 수확할 수 있습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n그로 미셀 바나나는 "송이" 단위로 수확하기 때문에, 다른 과일 나무들보다 빠르게 재배합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>그로 미셀 바나나는 캐번디시 바나나와는 다른 독특한 맛을 가지고 있습니다. 한때는 캐번디시 품종의 자리를 위협하기도 했었습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>달콤한 버찌를 맺는 벚꽃나무는 계절성 겨울철 시즌을 필요로 하는 것으로 유명합니다. 매우 아름다우며, 다양한 문화권에서 겨울 벚꽃축제의 무대가 되곤 합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n벚꽃나무는 다른 과일 나무보다 두배 아름답고, 겨울마다 만개하는 벚꽃으로 뒤덮입니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>붉은 열매로 점철된 낮게 자라는 덤불로, 고산지대 혹은 북위 38도 이상 고위도에서 쉽게 볼 수 있으며, 척박한 토양에서도 잘 자랍니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n월귤 덤불은 화분에서도 재배할 수 있습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>아삭아삭한 녹색 배입니다. 사과의 먼 사촌으로 서로 비슷하지만, 배가 섬유질이 더 많은 편이고 단맛이 덜합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>21세기를 강타한 대규모 바나나병 감염 사태에서 살아남은 품종으로 열대지방 대표적인 나무입니다. 노란색의 길쭉한 열매인 바나나가 따기 편하게 송이째로 달려 있습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n바나나는 한 번에 "송이"를 수확할 수 있어, 다른 나무들보다 수확 시간이 훨씬 짧습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>노란색의 길쭉한 열매로, 쉽게 껍질을 벗기면 매우 달고 무른 과육이 드러납니다. 이 열매는 수천 년 동안 열대 지방에서 인간과 다른 영장류 모두에게 사랑받아 왔습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>햇빛과 따뜻한 온도만 있다면 잘자라고, 솜털이 있는 예쁜 복숭아를 맺는 낙엽수입니다. 과거에도 인기가 많아 고대인들은 노란 문서에 복숭아 그림을 담아 서로 주고받았던 것으로 보입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n복숭아 나무는 매우 튼튼하여 자갈이 많은 지형에도 심을 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>raw dessert fruits</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1730,10 +1654,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>식물학적으로 가지과에 속하는 둥글고 부드러운 맛있는 검은 밤색 과일입니다. 따뜻한 날씨에서 잘 자랍니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 블랙뷰티 가지는 섭씨 37°C~60°C에서 30% 더 빨리 자랍니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>forage grass</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1770,22 +1690,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>재배된 사료용 풀입니다. 약간의 빛과 최소한의 양분만 있다면 어디서나 자라는 풀입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 건초와 마찬가지로 소에게 먹일 수 있습니다. 병충해의 영향을 받지 않지만, 건초처럼 수확하여 보관할 수는 없습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>재배된 사료용 키 큰 풀입니다. 통과할 때 느려지고, 약간의 빛과 최소한의 양분만 있다면 어디서나 자라는 풀입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 건초와 마찬가지로 소에게 먹일 수 있습니다. 병충해의 영향을 받지 않지만, 건초처럼 수확하여 보관할 수는 없습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>말 그대로 오렌지색의 이 열매는 껍질을 벗기기 어렵기로 악명이 높지만, 과육이 매우 많으며 상쾌한 단맛과 신맛이 나는 새콤달콤한 맛으로 유명합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>크고 무겁지만, 특유의 부드러운 단맛 덕분에 요리에 잘 사용되어 왔습니다. 다양한 문화권에서 식재료뿐만 아니라 할로윈 가면이나 잭 오 랜턴으로도 사용되었습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>작을 수록 매운 꼬투리로, 주로 소스나 가루로 낸 조미료로 사용됩니다. 자체적인 맛은 순하지만, 내부에 포함된 캡사이신 때문에 매운 맛을 느낄 수 있습니다.\n재배중일 때는 동물들이 먹지 않는 것으로 알려져 있습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1794,31 +1698,143 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>뿌리를 주로 먹으며 특유의 식감으로 사랑받는 채소 중 하나입니다. 당분 함량에 따라 다른 품종이 되기 때문에 같은 종인 사탕무는 설탕 생산원으로 길러집니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>식물학적으로 가지 식물은 가지과에 속하는 길다란 자주색 과일입니다. 따뜻한 날씨에서 잘 자랍니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 가지 식물은 온도가 37도에서 60도 사이일 때 30% 더 빠르게 자랍니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>원뿌리 식물인 비트는 허브 같은 식물로 사람과 가축을 위해 널리 재배됩니다. 특히 영양가가 높고 역사적으로는 염료 제조에 사용되곤 했습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 비트는 비옥한 토양을 필요로 하지만, 매우 튼튼하여 한겨울 동안에도 10%의 속도로 계속 자랄 수 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>덩굴식물로 자연에서는 땅바닥을 기면서 줄기에서 뿌리가 나와 자랍니다. 이 특징 덕에 뿌리째 뽑지 않고도 쉽게 덩굴에서 토마토를 수확할 수 있습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 토마토는 과일 나무처럼 수확해도 완전히 사라지지 않습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>직접 고안한 설명들이 있습니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>과거에 양배추를 독한 가루제의 농약을 뿌려가며 재배한 탓인지, 현재 이 품종은 공기 중 독소와 방사능에 대한 저항력이 매우 높습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 양배추는 유독성 낙진의 영향을 받지 않으며, 다른 식물과 달리 낙진으로 인해서는 죽지 않습니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>기술적으로 호박은 파종과 수확이 매우 쉬운 것으로 잘 알려져 있습니다. 상당한 내구성이 있지만, 크고 무거워서 수경재배기에 담기에는 너무 부담스럽습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 호박 수확은 재배 기술에 상관없이 항상 성공합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자주빛이 도는 붉은색의 달콤한 버찌입니다. 체리로도 불리는 버찌는 계절성 겨울 시즌이 필요하기 때문에, 추운 북방 문화권에서 인기 있는 과일이 되었습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>달콤한 버찌를 맺는 벚꽃나무는 계절성 겨울 시즌을 필요로 하는 것으로 유명합니다. 매우 아름다우며, 다양한 문화권에서 겨울 벚꽃축제의 무대가 되곤 합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n벚꽃나무는 다른 과일 나무보다 두배 아름답고, 겨울마다 만개하는 벚꽃으로 뒤덮입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤기 나고 맛있는 빨간 사과입니다. 사과는 인류 초기부터 간식, 디저트, 그리고 과일주를 만드는 데 사용되었습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>진한 보랏빛이 도는 매끈한 과일로 특히 신맛이 납니다. 다양하게 잼, 젤리, 과일주로 만들어 먹기도 하며, 장기 보존을 위해 말려서 건자두로 만들기도 합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt;상온에 두고 약 15일이 지나면 장기간 보관할 수 있는 말린 자두가 됩니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>프룬이라고도 불리는 건자두입니다. 오랫동안 상하지 않고 먹을 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>아삭아삭한 녹색 배입니다. 사과의 먼 사촌으로 비슷하지만, 배가 섬유질이 더 많은 편이고 단맛이 덜합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>작고 붉은 열매로 알려진 월귤입니다. 생으로 종종 먹을 때는 신맛과 밍밍한 맛이 나지만, 요리하면 자연스러운 단맛이 나오고 훨씬 더 맛있게 먹을 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>노란색의 길쭉한 열매로, 껍질을 벗기면 매우 달고 무른 과육이 드러납니다. 이 열매는 수천 년 동안 열대지방에서 인간과 다른 영장류 모두에게 사랑받아 왔습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>말 그대로 오렌지색의 이 열매는 껍질 벗기기가 어렵기로 악명 높지만, 과육이 매우 많으며 신맛과 상쾌한 단맛이 조화를 이루는 새콤달콤한 맛으로 유명합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>크고 무겁지만, 특유의 부드러운 단맛 덕분에 요리 재료로 잘 사용되어 왔습니다. 다양한 문화권에서 식재료뿐만 아니라 할로윈 가면이나 잭 오 랜턴으로도 사용되었습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>약간 단단한 잎이 많은 녹색 채소로, 그대로 조리하거나 종종 잘게 썰어 발효시켜 사용됩니다. 대표적인 요리로 샐러드와 코울슬로가 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>뿌리 부분을 주로 먹으며 특유의 식감 덕에 사랑받는 채소 중 하나입니다. 당분 함량에 따라서 다른 품종이 되기 때문에 같은 종인 사탕무는 설탕 생산원으로 길러집니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>즙이 많고 광택이 나는 연한 붉은 과일로, 일반적으로는 채소로 사용됩니다. 강하게 졸이면 내부의 산성이 부드러워져 감칠맛이 잘 느껴집니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>재배된 풀입니다. 약간의 빛과 최소한의 양분만 있다면 어디서나 자라는 풀입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 건초와 마찬가지로 가축의 주식으로 사용된다면 사실 잡초까지는 아닙니다. 병충해의 영향을 받지 않지만, 건초처럼 수확하여 보관할 수는 없습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>재배된 키 큰 풀입니다. 통과할 때 느려지고, 약간의 빛과 최소한의 양분만 있다면 어디서나 자라는 풀입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 건초와 마찬가지로 가축의 주식으로 사용된다면 사실 잡초까지는 아닙니다. 병충해의 영향을 받지 않지만, 건초처럼 수확하여 보관할 수는 없습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>완두는 물이 많이 필요하여 비가 오면 잘 자랍니다. 또한, 완두콩은 두꺼운 꼬투리 만큼 긴 보존 기간을 가지는 것으로 유명합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 평소에는 다른 작물보다 효율이 떨어지지만, 비가 올 때는 성장 속도가 50% 증가합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>원뿌리 식물인 비트는 사람과 가축을 위해 널리 재배됩니다. 영양가가 특히 높고 과거에는 염료 제조에 사용되곤 했습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 비트는 비옥한 토양을 필요로 하지만, 매우 튼튼하여 한겨울 동안에도 10%의 속도로 계속 자랄 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>영문 설명에 없던 내용들을 추가했습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사실 백년초 선인장은 잘못된 표현입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>림왈도에서 Grass는 잡초로 나옵니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>과채류가 어색하다면 과일로 롤백해주세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>덩굴식물로 땅바닥을 기면서 줄기로 뿌리가 나와 자랍니다. 이 특징 덕에 뿌리째 뽑지 않고도 쉽게 토마토를 수확할 수 있습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 토마토는 과일 나무처럼 수확해도 완전히 사라지지 않습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>윤기 나는 맛있는 빨간 사과를 맺는 나무로, 다양한 품종이 존재하지만 이 빨간 품종은 따뜻한 여름과 온화한 겨울을 선호합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>솜털이 있는 예쁜 복숭아를 맺는 낙엽수로, 햇빛과 따뜻한 온도만 있다면 잘 자랍니다. 이 나무들은 과거에도 인기가 많아 고대인들은 노란 문서에 복숭아 그림을 담아 서로 주고받았던 것으로 보입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n복숭아 나무는 매우 튼튼하여 자갈이 많은 지형에도 심을 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>21세기를 강타한 대규모 바나나병 감염 사태에서 살아남은 품종으로 열대지방 대표적인 파초입니다. 노란색의 길쭉한 열매인 바나나가 따기 편하게 송이째로 달려 있습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n바나나는 한 번에 "송이"를 수확할 수 있어, 다른 나무들보다 수확 시간이 훨씬 짧습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이 품종은 21세기에 멸종이 일어날 뻔한 대규모 바나나병 감염 사태에서도 살아남도록 유전자 변형되었습니다. 다른 바나나 나무처럼 한 번에 전체 "송이"를 수확할 수 있습니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 과일 나무는 일반 작물보다 약 4배의 공간을 더 차지하며, 열매를 맺는 데 오랜 시간이 걸립니다. 열매는 생으로 먹을 수 있으며, 수확해도 완전히 사라지지 않지만, 수명이 끝나면 새로 심어야 합니다.\n\n그로 미셀 바나나는 "송이" 단위로 수확하기 때문에, 다른 과일 나무들보다 빠르게 재배합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그로 미셀 바나나는 캐번디시 바나나와는 다른 독특한 맛을 가지고 있습니다. 한때는 이 세상의 모든 바나나 공급을 책임지기도 했었습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>식물학적으로 가지과에 속하는 둥글고 부드러운 맛있는 검은 밤색 과일입니다. 잘 자라기 위해선 따뜻한 날씨가 필요합니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 블랙뷰티 가지는 섭씨 37°C~60°C에서 30% 더 빨리 자랍니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>재배된 사료용 풀입니다. 약간의 빛과 최소한의 양분만 있다면 어디서나 자라는 풀입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 건초와 마찬가지로 가축이 먹을 수 있습니다. 병충해의 영향을 받지 않지만, 건초처럼 수확하여 보관할 수는 없습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>재배된 사료용 키 큰 풀입니다. 통과할 때 느려지고, 약간의 빛과 최소한의 양분만 있다면 어디서나 자라는 풀입니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt; 건초와 마찬가지로 가축이 먹을 수 있습니다. 병충해의 영향을 받지 않지만, 건초처럼 수확하여 보관할 수는 없습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>버찌 나무가 더 직관적이면 롤백해주세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>특유의 다소 떫은 맛을 가지고 있어 요리, 특히 과일 보존식품과 잼에 널리 사용됩니다. 많은 문화권에서는 자두를 건조하여 유통기한이 긴 말린 자두로 만듭니다.\n\n&amp;lt;color=#E5E54C&gt;특성:&amp;lt;/color&gt;상온에서 약 15일이 지나면 장기간 유통 가능한 말린 자두가 됩니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2221,7 +2237,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2231,7 +2249,7 @@
     <col min="4" max="4" width="24.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="64.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="53.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="39.85546875" style="4" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2255,7 +2273,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2323,7 +2341,10 @@
         <v>301</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>473</v>
+        <v>461</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -2357,7 +2378,7 @@
         <v>304</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>385</v>
+        <v>498</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2408,7 +2429,7 @@
         <v>307</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -2425,7 +2446,7 @@
         <v>308</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>382</v>
+        <v>496</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2459,7 +2480,7 @@
         <v>312</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>470</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2493,7 +2514,7 @@
         <v>314</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>337</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2527,7 +2548,7 @@
         <v>317</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>481</v>
+        <v>501</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2561,7 +2582,7 @@
         <v>320</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2595,7 +2616,7 @@
         <v>323</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>364</v>
+        <v>502</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2629,7 +2650,7 @@
         <v>325</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2663,7 +2684,7 @@
         <v>327</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2697,7 +2718,7 @@
         <v>329</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2731,7 +2752,7 @@
         <v>331</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2765,7 +2786,7 @@
         <v>333</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>515</v>
+        <v>491</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2785,7 +2806,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>79</v>
       </c>
@@ -2799,10 +2820,10 @@
         <v>335</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>81</v>
       </c>
@@ -2813,13 +2834,13 @@
         <v>82</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>83</v>
       </c>
@@ -2830,13 +2851,13 @@
         <v>84</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>85</v>
       </c>
@@ -2847,13 +2868,13 @@
         <v>86</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>87</v>
       </c>
@@ -2864,13 +2885,13 @@
         <v>88</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>89</v>
       </c>
@@ -2881,13 +2902,13 @@
         <v>90</v>
       </c>
       <c r="E38" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>91</v>
       </c>
@@ -2898,13 +2919,13 @@
         <v>92</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>93</v>
       </c>
@@ -2918,10 +2939,10 @@
         <v>95</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>96</v>
       </c>
@@ -2932,13 +2953,13 @@
         <v>97</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>98</v>
       </c>
@@ -2952,10 +2973,13 @@
         <v>100</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+        <v>355</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>101</v>
       </c>
@@ -2966,13 +2990,13 @@
         <v>102</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>103</v>
       </c>
@@ -2983,13 +3007,13 @@
         <v>104</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>105</v>
       </c>
@@ -3000,13 +3024,13 @@
         <v>106</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>107</v>
       </c>
@@ -3017,13 +3041,13 @@
         <v>108</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>109</v>
       </c>
@@ -3034,13 +3058,13 @@
         <v>110</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>111</v>
       </c>
@@ -3051,7 +3075,7 @@
         <v>112</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>328</v>
@@ -3068,10 +3092,10 @@
         <v>114</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -3085,7 +3109,7 @@
         <v>116</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>330</v>
@@ -3102,10 +3126,10 @@
         <v>118</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>523</v>
+        <v>495</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -3136,10 +3160,10 @@
         <v>123</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -3153,10 +3177,10 @@
         <v>125</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -3170,10 +3194,10 @@
         <v>127</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>391</v>
+        <v>511</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -3190,7 +3214,7 @@
         <v>130</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -3204,10 +3228,10 @@
         <v>132</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>518</v>
+        <v>493</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3224,7 +3248,7 @@
         <v>135</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -3238,10 +3262,10 @@
         <v>137</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>522</v>
+        <v>494</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -3258,7 +3282,7 @@
         <v>140</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -3272,10 +3296,10 @@
         <v>142</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -3292,7 +3316,7 @@
         <v>145</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -3306,10 +3330,10 @@
         <v>147</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -3326,10 +3350,10 @@
         <v>150</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>151</v>
       </c>
@@ -3340,13 +3364,13 @@
         <v>152</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>153</v>
       </c>
@@ -3360,10 +3384,10 @@
         <v>155</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>156</v>
       </c>
@@ -3374,13 +3398,13 @@
         <v>157</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>158</v>
       </c>
@@ -3394,10 +3418,13 @@
         <v>160</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>161</v>
       </c>
@@ -3408,13 +3435,13 @@
         <v>162</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>163</v>
       </c>
@@ -3428,10 +3455,10 @@
         <v>165</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>166</v>
       </c>
@@ -3442,13 +3469,13 @@
         <v>167</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>168</v>
       </c>
@@ -3459,13 +3486,13 @@
         <v>169</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>170</v>
       </c>
@@ -3476,13 +3503,13 @@
         <v>171</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>172</v>
       </c>
@@ -3493,13 +3520,16 @@
         <v>173</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>174</v>
       </c>
@@ -3510,13 +3540,13 @@
         <v>175</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>176</v>
       </c>
@@ -3527,13 +3557,13 @@
         <v>177</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>178</v>
       </c>
@@ -3544,13 +3574,13 @@
         <v>179</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>180</v>
       </c>
@@ -3564,10 +3594,10 @@
         <v>182</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>183</v>
       </c>
@@ -3578,13 +3608,13 @@
         <v>184</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>185</v>
       </c>
@@ -3598,7 +3628,7 @@
         <v>187</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3612,10 +3642,10 @@
         <v>189</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3629,10 +3659,10 @@
         <v>192</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3649,10 +3679,10 @@
         <v>196</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3669,7 +3699,7 @@
         <v>199</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3686,7 +3716,7 @@
         <v>193</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3703,10 +3733,10 @@
         <v>196</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3723,7 +3753,7 @@
         <v>199</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3740,7 +3770,7 @@
         <v>193</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>509</v>
+        <v>489</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3757,10 +3787,10 @@
         <v>196</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>508</v>
+        <v>488</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>510</v>
+        <v>490</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3777,7 +3807,7 @@
         <v>199</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3794,7 +3824,7 @@
         <v>215</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3811,7 +3841,7 @@
         <v>218</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3828,7 +3858,7 @@
         <v>221</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3845,7 +3875,7 @@
         <v>224</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3862,10 +3892,10 @@
         <v>227</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -3882,10 +3912,10 @@
         <v>227</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
@@ -3905,7 +3935,7 @@
         <v>230</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
@@ -3922,10 +3952,10 @@
         <v>227</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
@@ -3942,10 +3972,10 @@
         <v>227</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3962,10 +3992,10 @@
         <v>227</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -3985,7 +4015,7 @@
         <v>235</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -4002,10 +4032,10 @@
         <v>227</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
@@ -4022,10 +4052,10 @@
         <v>227</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
@@ -4042,10 +4072,10 @@
         <v>227</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
@@ -4065,7 +4095,7 @@
         <v>240</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
@@ -4085,7 +4115,7 @@
         <v>242</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -4102,10 +4132,10 @@
         <v>227</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -4122,10 +4152,10 @@
         <v>227</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -4145,7 +4175,7 @@
         <v>246</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -4165,7 +4195,7 @@
         <v>248</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -4182,10 +4212,10 @@
         <v>227</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
@@ -4202,10 +4232,10 @@
         <v>227</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>463</v>
+        <v>453</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
@@ -4222,10 +4252,10 @@
         <v>227</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>486</v>
+        <v>467</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
@@ -4245,7 +4275,7 @@
         <v>253</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -4262,10 +4292,10 @@
         <v>227</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -4282,10 +4312,10 @@
         <v>227</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
@@ -4305,7 +4335,7 @@
         <v>257</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -4322,10 +4352,10 @@
         <v>227</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>456</v>
+        <v>446</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -4342,10 +4372,10 @@
         <v>227</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>443</v>
+        <v>433</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
@@ -4362,10 +4392,10 @@
         <v>227</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
@@ -4385,7 +4415,7 @@
         <v>262</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
@@ -4402,10 +4432,10 @@
         <v>227</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
@@ -4425,7 +4455,7 @@
         <v>265</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
@@ -4442,10 +4472,10 @@
         <v>227</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
@@ -4462,10 +4492,10 @@
         <v>227</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>455</v>
+        <v>445</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
@@ -4482,10 +4512,10 @@
         <v>227</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
@@ -4502,10 +4532,10 @@
         <v>227</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>466</v>
+        <v>456</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -4522,10 +4552,10 @@
         <v>227</v>
       </c>
       <c r="E128" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="F128" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
@@ -4545,7 +4575,7 @@
         <v>272</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -4565,7 +4595,7 @@
         <v>274</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>469</v>
+        <v>527</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
@@ -4582,10 +4612,10 @@
         <v>227</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>471</v>
+        <v>459</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
@@ -4602,10 +4632,10 @@
         <v>227</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>472</v>
+        <v>460</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>477</v>
+        <v>521</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
@@ -4622,10 +4652,10 @@
         <v>227</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>474</v>
+        <v>462</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>475</v>
+        <v>463</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
@@ -4645,7 +4675,7 @@
         <v>279</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>478</v>
+        <v>522</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
@@ -4662,10 +4692,10 @@
         <v>227</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>485</v>
+        <v>466</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>487</v>
+        <v>468</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
@@ -4682,10 +4712,10 @@
         <v>283</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>488</v>
+        <v>469</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>492</v>
+        <v>473</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
@@ -4702,10 +4732,10 @@
         <v>283</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>490</v>
+        <v>471</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -4722,10 +4752,10 @@
         <v>283</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>489</v>
+        <v>470</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.3">
@@ -4742,10 +4772,10 @@
         <v>283</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>491</v>
+        <v>472</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>493</v>
+        <v>474</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
@@ -4762,10 +4792,10 @@
         <v>283</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
@@ -4782,10 +4812,10 @@
         <v>283</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>501</v>
+        <v>523</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
@@ -4805,7 +4835,7 @@
         <v>290</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
@@ -4822,10 +4852,10 @@
         <v>283</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>498</v>
+        <v>479</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
@@ -4842,10 +4872,10 @@
         <v>283</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>502</v>
+        <v>482</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>506</v>
+        <v>486</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
@@ -4862,10 +4892,10 @@
         <v>283</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>505</v>
+        <v>485</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>507</v>
+        <v>487</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
@@ -4882,10 +4912,10 @@
         <v>283</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>503</v>
+        <v>483</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>511</v>
+        <v>524</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -4902,10 +4932,10 @@
         <v>283</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>504</v>
+        <v>484</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>512</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>